<commit_message>
created a new figures folder and added figure to it
</commit_message>
<xml_diff>
--- a/data/contracts.xlsx
+++ b/data/contracts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmage\Desktop\MATH_437_FP\hockey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F19AC85-7FC3-404E-AE46-038CA05F7A06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02629B2-0EBC-4E72-92F3-D440D8D6AB6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5546,7 +5546,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A295" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A295" sqref="A295"/>
+      <selection pane="bottomLeft" activeCell="J303" sqref="J303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>